<commit_message>
update bar plot with production costs
</commit_message>
<xml_diff>
--- a/Plotting/production_shares_ammonia.xlsx
+++ b/Plotting/production_shares_ammonia.xlsx
@@ -535,7 +535,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1184000.000000012</v>
+        <v>1184000.000000039</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -588,10 +588,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1177703.720175931</v>
+        <v>1177703.294781314</v>
       </c>
       <c r="G6" t="n">
-        <v>1155650.958798334</v>
+        <v>1155650.958798337</v>
       </c>
     </row>
     <row r="7">
@@ -616,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>22047.650537326</v>
+        <v>22047.71408006548</v>
       </c>
     </row>
     <row r="8">

</xml_diff>